<commit_message>
Fixed Asset Depreciation Code change
</commit_message>
<xml_diff>
--- a/SmokeSuite/TestResource/EnvParamaters.xlsx
+++ b/SmokeSuite/TestResource/EnvParamaters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Wpp_Project_Final\Wpp_Project\wppGTCRegressionAutomation\SmokeSuite\TestResource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\674087\Documents\China\GlobalTestPack\SmokeSuite\TestResource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6420" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6420" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CountryMapping" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="176">
   <si>
     <t>InstanceToRun</t>
   </si>
@@ -122,21 +122,9 @@
     <t>Test Summary</t>
   </si>
   <si>
-    <t>JobCreation</t>
-  </si>
-  <si>
     <t>TSTAUTO-1</t>
   </si>
   <si>
-    <t>Timesheet</t>
-  </si>
-  <si>
-    <t>CreateExpenses</t>
-  </si>
-  <si>
-    <t>EmployeeCreation</t>
-  </si>
-  <si>
     <t>CreateUser</t>
   </si>
   <si>
@@ -546,6 +534,30 @@
   </si>
   <si>
     <t>bauapac</t>
+  </si>
+  <si>
+    <t>QueryAndValidateExistingJob</t>
+  </si>
+  <si>
+    <t>QueryAndValidateExistingEmployee</t>
+  </si>
+  <si>
+    <t>PrintJobBudgetMPL</t>
+  </si>
+  <si>
+    <t>VerfiyTimesheet</t>
+  </si>
+  <si>
+    <t>TSTAUTO-73</t>
+  </si>
+  <si>
+    <t>TSTAUTO-74</t>
+  </si>
+  <si>
+    <t>TSTAUTO-75</t>
+  </si>
+  <si>
+    <t>TSTAUTO-76</t>
   </si>
 </sst>
 </file>
@@ -757,7 +769,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -797,6 +809,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1159,14 +1172,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1181,1070 +1195,1070 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>30</v>
+      <c r="A2" s="21" t="s">
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>32</v>
+      <c r="A3" s="21" t="s">
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>173</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>33</v>
+      <c r="A4" s="21" t="s">
+        <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>172</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>34</v>
+      <c r="A5" s="21" t="s">
+        <v>171</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>175</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C58" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B59" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C59" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B60" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C60" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B62" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C62" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B63" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C63" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B67" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C67" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B68" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C68" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B69" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C69" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B70" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C70" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B72" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C72" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B73" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C73" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B74" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C74" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B75" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C75" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B76" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C76" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B77" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C77" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B78" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C78" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B79" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C79" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B80" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C80" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B81" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C81" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B82" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C82" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B83" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C83" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B84" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C84" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B85" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C85" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B86" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C86" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B87" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C87" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B88" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C88" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B89" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C89" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B90" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C90" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B91" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C91" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B92" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C92" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B93" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C93" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B94" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C94" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B95" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C95" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B96" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C96" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B98" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C98" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2271,7 +2285,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2279,7 +2293,7 @@
         <v>1201</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2287,7 +2301,7 @@
         <v>1322</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2295,7 +2309,7 @@
         <v>1314</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2303,7 +2317,7 @@
         <v>1319</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2311,7 +2325,7 @@
         <v>1307</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2319,7 +2333,7 @@
         <v>1204</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2327,7 +2341,7 @@
         <v>1213</v>
       </c>
       <c r="B8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2335,7 +2349,7 @@
         <v>1284</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2343,7 +2357,7 @@
         <v>1271</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2351,7 +2365,7 @@
         <v>1205</v>
       </c>
       <c r="B11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2359,7 +2373,7 @@
         <v>1240</v>
       </c>
       <c r="B12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2367,7 +2381,7 @@
         <v>1228</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2375,7 +2389,7 @@
         <v>1315</v>
       </c>
       <c r="B14" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2383,7 +2397,7 @@
         <v>1309</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2391,7 +2405,7 @@
         <v>1318</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2399,7 +2413,7 @@
         <v>1321</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2407,7 +2421,7 @@
         <v>1301</v>
       </c>
       <c r="B18" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2415,7 +2429,7 @@
         <v>1295</v>
       </c>
       <c r="B19" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2423,7 +2437,7 @@
         <v>1289</v>
       </c>
       <c r="B20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2431,7 +2445,7 @@
         <v>1216</v>
       </c>
       <c r="B21" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2439,7 +2453,7 @@
         <v>1285</v>
       </c>
       <c r="B22" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2447,7 +2461,7 @@
         <v>1273</v>
       </c>
       <c r="B23" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2455,7 +2469,7 @@
         <v>1269</v>
       </c>
       <c r="B24" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2463,7 +2477,7 @@
         <v>1263</v>
       </c>
       <c r="B25" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2471,7 +2485,7 @@
         <v>1221</v>
       </c>
       <c r="B26" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2479,7 +2493,7 @@
         <v>1253</v>
       </c>
       <c r="B27" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2487,7 +2501,7 @@
         <v>1203</v>
       </c>
       <c r="B28" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2495,7 +2509,7 @@
         <v>1246</v>
       </c>
       <c r="B29" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2503,7 +2517,7 @@
         <v>1229</v>
       </c>
       <c r="B30" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2511,7 +2525,7 @@
         <v>1239</v>
       </c>
       <c r="B31" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2519,7 +2533,7 @@
         <v>1296</v>
       </c>
       <c r="B32" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2527,7 +2541,7 @@
         <v>1304</v>
       </c>
       <c r="B33" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2535,7 +2549,7 @@
         <v>1214</v>
       </c>
       <c r="B34" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2543,7 +2557,7 @@
         <v>1330</v>
       </c>
       <c r="B35" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2569,29 +2583,29 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>12</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B3" s="20">
         <v>443</v>
@@ -2602,13 +2616,13 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2625,8 +2639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2766,6 +2780,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BF89F52BC52D9844A146207839183849" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aeefbe4ea6f9147130b7e91bb765e7bf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="685ce2a4-4455-466c-aa76-63e1d1928dc9" xmlns:ns3="b437d513-bcd3-4295-b540-77b94a32e6f7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c60527f9dafc4da954eac34746def061" ns2:_="" ns3:_="">
     <xsd:import namespace="685ce2a4-4455-466c-aa76-63e1d1928dc9"/>
@@ -2962,22 +2991,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52A13E29-6E7D-4EFA-ADA2-5464726AEB4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BC53470-14F7-4B25-B9BE-408A8E1FA143}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B25B39F-B7E2-4EE4-BA95-48E33E44BF6E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2994,21 +3025,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BC53470-14F7-4B25-B9BE-408A8E1FA143}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52A13E29-6E7D-4EFA-ADA2-5464726AEB4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>